<commit_message>
updated base mapping file
</commit_message>
<xml_diff>
--- a/termREN/2023/TERMREN_mapping_2023.xlsx
+++ b/termREN/2023/TERMREN_mapping_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAVIDSONKA\Documents\ANALYSIS\WCVI_Chinook_Term_Run_Recon\WCVI_CN_TermRunRecon\termREN\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE7250C-6E19-4DDD-9B84-EA5FB66D1DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF791A2-D605-45CF-89BD-73050AFC0ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="1" xr2:uid="{E2731BFC-E1F4-4F7A-AD91-46B95AB44FF5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{E2731BFC-E1F4-4F7A-AD91-46B95AB44FF5}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -378,7 +378,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="89">
   <si>
     <t>Recreational</t>
   </si>
@@ -419,9 +419,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>June, July</t>
-  </si>
-  <si>
     <t>Enumeration</t>
   </si>
   <si>
@@ -441,12 +438,6 @@
   </si>
   <si>
     <t>TermRun_subgroup_AGESspat</t>
-  </si>
-  <si>
-    <t>21A,121C</t>
-  </si>
-  <si>
-    <t>June,July</t>
   </si>
   <si>
     <t>Broodstock, morts, other</t>
@@ -648,6 +639,12 @@
   </si>
   <si>
     <t>20A, 20B, 20E</t>
+  </si>
+  <si>
+    <t>June, July, August, September</t>
+  </si>
+  <si>
+    <t>In-River</t>
   </si>
 </sst>
 </file>
@@ -1106,77 +1103,77 @@
   <sheetData>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B5" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>28</v>
+      <c r="B9" t="s">
+        <v>38</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>34</v>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>43</v>
-      </c>
       <c r="L11" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
@@ -1186,13 +1183,13 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
@@ -1202,13 +1199,13 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L13" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
@@ -1218,13 +1215,13 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
@@ -1234,13 +1231,13 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
@@ -50374,8 +50371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD15511-D0E0-440B-B215-63E04B9AC67B}">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50404,72 +50401,72 @@
   <sheetData>
     <row r="1" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>76</v>
+      <c r="N2" s="2" t="s">
+        <v>45</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>63</v>
+      <c r="O2" s="2" t="s">
+        <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="P2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>27</v>
+      <c r="Q2" s="2" t="s">
+        <v>47</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="N2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="S2" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -50477,16 +50474,16 @@
         <v>2023</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>11</v>
@@ -50495,31 +50492,31 @@
         <v>20</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="P3" s="4">
         <v>2023</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="S3" s="4">
         <v>2022</v>
@@ -50530,16 +50527,16 @@
         <v>2023</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>12</v>
@@ -50548,31 +50545,31 @@
         <v>20</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="P4" s="4">
         <v>2023</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="S4" s="4">
         <v>2022</v>
@@ -50583,16 +50580,16 @@
         <v>2023</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>7</v>
@@ -50601,34 +50598,34 @@
         <v>20</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J5" s="4">
         <v>10</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="P5" s="4">
         <v>2023</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="S5" s="4">
         <v>2022</v>
@@ -50639,46 +50636,46 @@
         <v>2023</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P6" s="4">
         <v>2023</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S6" s="4">
         <v>2022</v>
@@ -50689,46 +50686,46 @@
         <v>2023</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P7" s="4">
         <v>2023</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S7" s="4">
         <v>2022</v>
@@ -50739,49 +50736,49 @@
         <v>2023</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J8" s="4">
         <v>5</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P8" s="4">
         <v>2023</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S8" s="4">
         <v>2022</v>
@@ -50792,44 +50789,44 @@
         <v>2023</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H9" s="3">
         <v>20</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="O9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P9" s="8"/>
       <c r="Q9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -50837,13 +50834,13 @@
         <v>2023</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>8</v>
@@ -50852,26 +50849,26 @@
         <v>20</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
       <c r="O10" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P10" s="8"/>
       <c r="Q10" s="4" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="S10" s="4">
         <v>2022</v>
@@ -50882,13 +50879,13 @@
         <v>2023</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>9</v>
@@ -50897,26 +50894,26 @@
         <v>20</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
       <c r="O11" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P11" s="8"/>
       <c r="Q11" s="4" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="S11" s="4">
         <v>2022</v>
@@ -50927,13 +50924,13 @@
         <v>2023</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>10</v>
@@ -50942,29 +50939,29 @@
         <v>20</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
       <c r="O12" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P12" s="8"/>
       <c r="Q12" s="4" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
-      <c r="S12" s="4" t="s">
-        <v>16</v>
+      <c r="S12" s="4">
+        <v>2022</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -50972,13 +50969,13 @@
         <v>2023</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>9</v>
@@ -50987,28 +50984,28 @@
         <v>0</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P13" s="4">
         <v>2023</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S13" s="4">
         <v>2022</v>
@@ -51019,13 +51016,13 @@
         <v>2023</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>10</v>
@@ -51034,28 +51031,28 @@
         <v>0</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P14" s="4">
         <v>2023</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S14" s="4">
         <v>2022</v>
@@ -51066,7 +51063,7 @@
         <v>2023</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>1</v>
@@ -51075,43 +51072,43 @@
         <v>2</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H15" s="3">
         <v>20</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J15" s="4">
         <v>0</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -51119,7 +51116,7 @@
         <v>2023</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>1</v>
@@ -51128,43 +51125,43 @@
         <v>3</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H16" s="3">
         <v>20</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="J16" s="4">
         <v>0</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -51172,49 +51169,49 @@
         <v>2023</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J17" s="4">
         <v>210</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="P17" s="4">
         <v>2023</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R17" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S17" s="4">
         <v>2022</v>
@@ -51225,49 +51222,49 @@
         <v>2023</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J18" s="4">
         <v>155</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="P18" s="4">
         <v>2023</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R18" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S18" s="4">
         <v>2022</v>
@@ -51278,49 +51275,49 @@
         <v>2023</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J19" s="4">
         <v>1</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="P19" s="4">
         <v>2023</v>
       </c>
       <c r="Q19" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S19" s="4">
         <v>2022</v>
@@ -51331,49 +51328,49 @@
         <v>2023</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J20" s="4">
         <v>0</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="P20" s="4">
         <v>2023</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R20" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S20" s="4">
         <v>2022</v>
@@ -51384,7 +51381,7 @@
         <v>2023</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>5</v>
@@ -51393,40 +51390,40 @@
         <v>4</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J21" s="4">
         <v>2597</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P21" s="4">
         <v>2023</v>
       </c>
       <c r="Q21" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S21" s="4">
         <v>2022</v>
@@ -51437,7 +51434,7 @@
         <v>2023</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>5</v>
@@ -51446,40 +51443,40 @@
         <v>4</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J22" s="4">
         <v>2664</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P22" s="4">
         <v>2023</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S22" s="4">
         <v>2022</v>
@@ -51490,7 +51487,7 @@
         <v>2023</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>6</v>
@@ -51499,40 +51496,40 @@
         <v>4</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J23" s="4">
         <v>21</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P23" s="4">
         <v>2023</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R23" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S23" s="4">
         <v>2022</v>
@@ -51543,7 +51540,7 @@
         <v>2023</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>6</v>
@@ -51552,40 +51549,40 @@
         <v>4</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J24" s="4">
         <v>24</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P24" s="4">
         <v>2023</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R24" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S24" s="4">
         <v>2022</v>
@@ -51596,7 +51593,7 @@
         <v>2023</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>6</v>
@@ -51605,40 +51602,40 @@
         <v>4</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J25" s="4">
         <v>77</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P25" s="4">
         <v>2023</v>
       </c>
       <c r="Q25" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R25" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S25" s="4">
         <v>2022</v>
@@ -51649,7 +51646,7 @@
         <v>2023</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>6</v>
@@ -51658,40 +51655,40 @@
         <v>4</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J26" s="4">
         <v>14</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P26" s="4">
         <v>2023</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R26" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S26" s="4">
         <v>2022</v>
@@ -51702,7 +51699,7 @@
         <v>2023</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>6</v>
@@ -51711,40 +51708,40 @@
         <v>4</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J27" s="4">
         <v>0</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O27" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="P27" s="4">
         <v>2023</v>
       </c>
       <c r="Q27" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R27" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="S27" s="4">
         <v>2022</v>
@@ -51755,49 +51752,49 @@
         <v>2023</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="J28" s="7">
-        <v>0.75</v>
+        <v>0.753</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O28" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="P28" s="4">
         <v>2023</v>
       </c>
       <c r="Q28" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R28" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S28" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -51805,16 +51802,16 @@
         <v>2023</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>12</v>
@@ -51823,31 +51820,31 @@
         <v>0.23</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="P29" s="4">
         <v>2023</v>
       </c>
       <c r="Q29" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R29" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S29" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -51855,49 +51852,49 @@
         <v>2023</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J30" s="7">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O30" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="P30" s="4">
         <v>2023</v>
       </c>
       <c r="Q30" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="R30" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S30" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>